<commit_message>
update task to do
</commit_message>
<xml_diff>
--- a/Documents/Task to do.xlsx
+++ b/Documents/Task to do.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My_Work\Generator_ReactiveForm\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My_Work\Generator_ReactiveForm\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A71EF26D-6BF0-4828-8151-C8665B8CBFB8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D23713E-46B7-4B65-957F-E091F62E95F9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{ACBE65D1-08DE-4AB2-8803-F82446C36B7C}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Task</t>
   </si>
@@ -64,6 +64,18 @@
   </si>
   <si>
     <t>ratio</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Research drag drop</t>
+  </si>
+  <si>
+    <t>DONE</t>
+  </si>
+  <si>
+    <t>status</t>
   </si>
 </sst>
 </file>
@@ -79,12 +91,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -99,8 +123,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,60 +441,97 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D20D59B-A7B4-4D76-906A-DFC20212855B}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.21875" customWidth="1"/>
+    <col min="2" max="2" width="31.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>7</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>8</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>9</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6">
         <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>